<commit_message>
♻️ refactor(examples): improve example file generation
- update `generate_example_files.py` to streamline logic
- remove redundant functions and simplify data generation
- enhance data generation in `CustomerData` and `Transactions` sheets

✨ feat(rules): add rule executor for migration tasks

- introduce `RuleExecutor` class to execute Excel migration rules
- implement field mapping and calculation execution logic

♻️ refactor(rules): enhance rule engine for better execution

- update `RuleEngine` to support rule execution with `RuleExecutor`
- refine rule generation logic and integrate loguru for logging

✨ feat(testing): extend rule testing with executor integration

- add `RuleExecutor` to `generate_and_test_rules` context
- update testing workflow to validate execution of rules through executor
</commit_message>
<xml_diff>
--- a/examples/data/target.xlsx
+++ b/examples/data/target.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -26,22 +26,13 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b val="1"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0092D050"/>
-        <bgColor rgb="0092D050"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -56,12 +47,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -427,147 +414,53 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="13" customWidth="1" min="2" max="2"/>
-    <col width="49" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="34" customWidth="1" min="5" max="5"/>
-    <col width="8" customWidth="1" min="6" max="6"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>CustomerID</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>FullName</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>ContactInfo</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>MemberSince</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>PurchaseMetrics</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1001</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>Email: john.doe@email.com
-Phone: 123-456-7890</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>January 2023</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>Total: $1,250.50
-Transactions: 2</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1002</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Jane Smith</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>Email: jane.smith@email.com
-Phone: 234-567-8901</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>February 2023</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>Total: $2,100.75
-Transactions: 1</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1003</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Bob Johnson</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>Email: bob.j@email.com
-Phone: 345-678-9012</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>March 2023</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="inlineStr">
-        <is>
-          <t>Total: $750.25
-Transactions: 1</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Active</t>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>DaysSinceRegistration</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>LastLoginDate</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>IsActive</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>TransactionCount</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>TotalSpent</t>
         </is>
       </c>
     </row>
@@ -582,179 +475,43 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="13" customWidth="1" min="2" max="2"/>
-    <col width="14" customWidth="1" min="3" max="3"/>
-    <col width="9" customWidth="1" min="4" max="4"/>
-    <col width="18" customWidth="1" min="5" max="5"/>
-    <col width="13" customWidth="1" min="6" max="6"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>TransactionID</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Customer</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Product</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>OrderDetails</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>CustomerID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>TransactionCount</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
         <is>
           <t>TotalAmount</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>T001</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Jun 1, 2023</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>P101</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2 units @ $25.99</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>$51.98</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>T002</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Jun 15, 2023</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>P102</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>1 unit @ $99.99</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>$99.99</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>T003</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Jane Smith</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Jun 20, 2023</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>P101</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>3 units @ $25.99</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>$77.97</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>T004</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Bob Johnson</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Jun 25, 2023</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>P103</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>1 unit @ $149.99</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>$149.99</t>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>AverageAmount</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>LastTransactionDate</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>SuccessRate</t>
         </is>
       </c>
     </row>

</xml_diff>